<commit_message>
removing test dialogs and testing with more movies
</commit_message>
<xml_diff>
--- a/Files/Movie-Data.xlsx
+++ b/Files/Movie-Data.xlsx
@@ -1,81 +1,135 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
-  <workbookPr codeName="ThisWorkbook"/>
+<x:workbook xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <x:fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
+  <x:workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jaskaran\Documents\UiPath\RPA-G4-2023\Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AEC33B3-EE51-49A3-922F-CDBB5EE5076F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
-  </bookViews>
-  <sheets>
-    <sheet name="details" sheetId="1" r:id="rId1"/>
-  </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <x:bookViews>
+    <x:workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" firstSheet="0" activeTab="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </x:bookViews>
+  <x:sheets>
+    <x:sheet name="details" sheetId="1" r:id="rId1"/>
+  </x:sheets>
+  <x:definedNames/>
+  <x:calcPr calcId="162913"/>
+  <x:extLst>
+    <x:ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
-</workbook>
+    </x:ext>
+  </x:extLst>
+</x:workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+  <x:si>
+    <x:t>Name</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Rating</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Budget</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Domestic Revenue</x:t>
+  </x:si>
+  <x:si>
+    <x:t>International Revenue</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Worldwide Revenue</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Inception</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Jarhead</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Man of Steel</x:t>
+  </x:si>
+  <x:si>
+    <x:t>The Avengers</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Avengers: Age of Ultron</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Interstellar</x:t>
+  </x:si>
+</x:sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-  </fonts>
-  <fills count="2">
-    <fill>
-      <patternFill patternType="none"/>
-    </fill>
-    <fill>
-      <patternFill patternType="gray125"/>
-    </fill>
-  </fills>
-  <borders count="1">
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-  </borders>
-  <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-  </cellStyleXfs>
-  <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-  </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-  </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+<x:styleSheet xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x14ac x16r2 xr">
+  <x:numFmts count="1">
+    <x:numFmt numFmtId="0" formatCode=""/>
+  </x:numFmts>
+  <x:fonts count="2" x14ac:knownFonts="1">
+    <x:font>
+      <x:sz val="11"/>
+      <x:color theme="1"/>
+      <x:name val="Calibri"/>
+      <x:family val="2"/>
+      <x:scheme val="minor"/>
+    </x:font>
+    <x:font>
+      <x:vertAlign val="baseline"/>
+      <x:sz val="11"/>
+      <x:color rgb="FF000000"/>
+      <x:name val="Calibri"/>
+      <x:family val="2"/>
+    </x:font>
+  </x:fonts>
+  <x:fills count="2">
+    <x:fill>
+      <x:patternFill patternType="none"/>
+    </x:fill>
+    <x:fill>
+      <x:patternFill patternType="gray125"/>
+    </x:fill>
+  </x:fills>
+  <x:borders count="1">
+    <x:border>
+      <x:left/>
+      <x:right/>
+      <x:top/>
+      <x:bottom/>
+      <x:diagonal/>
+    </x:border>
+  </x:borders>
+  <x:cellStyleXfs count="2">
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+  </x:cellStyleXfs>
+  <x:cellXfs count="2">
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+  </x:cellXfs>
+  <x:cellStyles count="1">
+    <x:cellStyle name="Normal" xfId="0" builtinId="0"/>
+  </x:cellStyles>
+  <x:tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <x:extLst>
+    <x:ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+    </x:ext>
+    <x:ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
       <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
-</styleSheet>
+    </x:ext>
+  </x:extLst>
+</x:styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -340,23 +394,171 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="A1:F3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="19.42578125" customWidth="1"/>
-    <col min="2" max="2" width="23.42578125" customWidth="1"/>
-    <col min="3" max="3" width="35.85546875" customWidth="1"/>
-    <col min="4" max="4" width="36.28515625" customWidth="1"/>
-    <col min="5" max="5" width="25.5703125" customWidth="1"/>
-    <col min="6" max="6" width="27.28515625" customWidth="1"/>
-  </cols>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xr:uid="{00000000-0001-0000-0000-000000000000}" mc:Ignorable="x14ac xr xr2 xr3">
+  <x:sheetPr>
+    <x:outlinePr summaryBelow="1" summaryRight="1"/>
+  </x:sheetPr>
+  <x:dimension ref="A1"/>
+  <x:sheetViews>
+    <x:sheetView tabSelected="1" workbookViewId="0">
+      <x:selection activeCell="F3" sqref="F3 A1:F3"/>
+    </x:sheetView>
+  </x:sheetViews>
+  <x:sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <x:cols>
+    <x:col min="1" max="1" width="19.425781" style="1" customWidth="1"/>
+    <x:col min="2" max="2" width="23.425781" style="1" customWidth="1"/>
+    <x:col min="3" max="3" width="35.855469" style="1" customWidth="1"/>
+    <x:col min="4" max="4" width="36.285156" style="1" customWidth="1"/>
+    <x:col min="5" max="5" width="25.570312" style="1" customWidth="1"/>
+    <x:col min="6" max="6" width="27.285156" style="1" customWidth="1"/>
+  </x:cols>
+  <x:sheetData>
+    <x:row r="1" spans="1:6">
+      <x:c r="A1" s="1" t="s">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="B1" s="1" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C1" s="1" t="s">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="D1" s="1" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="E1" s="1" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="F1" s="1" t="s">
+        <x:v>5</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2" spans="1:6">
+      <x:c r="A2" s="1" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="B2" s="1" t="n">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="C2" s="1" t="n">
+        <x:v>160000000</x:v>
+      </x:c>
+      <x:c r="D2" s="1" t="n">
+        <x:v>292587330</x:v>
+      </x:c>
+      <x:c r="E2" s="1" t="n">
+        <x:v>544599280</x:v>
+      </x:c>
+      <x:c r="F2" s="1" t="n">
+        <x:v>837186610</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="3" spans="1:6">
+      <x:c r="A3" s="1" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="B3" s="1" t="n">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="C3" s="1" t="n">
+        <x:v>72000000</x:v>
+      </x:c>
+      <x:c r="D3" s="1" t="n">
+        <x:v>62658220</x:v>
+      </x:c>
+      <x:c r="E3" s="1" t="n">
+        <x:v>34417932</x:v>
+      </x:c>
+      <x:c r="F3" s="1" t="n">
+        <x:v>97076152</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="4" spans="1:6">
+      <x:c r="A4" s="1" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="B4" s="1" t="n">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="C4" s="1" t="n">
+        <x:v>225000000</x:v>
+      </x:c>
+      <x:c r="D4" s="1" t="n">
+        <x:v>291045518</x:v>
+      </x:c>
+      <x:c r="E4" s="1" t="n">
+        <x:v>377000000</x:v>
+      </x:c>
+      <x:c r="F4" s="1" t="n">
+        <x:v>668045518</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="5" spans="1:6">
+      <x:c r="A5" s="1" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="B5" s="1" t="n">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="C5" s="1" t="n">
+        <x:v>220000000</x:v>
+      </x:c>
+      <x:c r="D5" s="1" t="n">
+        <x:v>623357910</x:v>
+      </x:c>
+      <x:c r="E5" s="1" t="n">
+        <x:v>897180626</x:v>
+      </x:c>
+      <x:c r="F5" s="1" t="n">
+        <x:v>1520538536</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="6" spans="1:6">
+      <x:c r="A6" s="1" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="B6" s="1" t="n">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="C6" s="1" t="n">
+        <x:v>250000000</x:v>
+      </x:c>
+      <x:c r="D6" s="1" t="n">
+        <x:v>459005868</x:v>
+      </x:c>
+      <x:c r="E6" s="1" t="n">
+        <x:v>946012180</x:v>
+      </x:c>
+      <x:c r="F6" s="1" t="n">
+        <x:v>1405018048</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="7" spans="1:6">
+      <x:c r="A7" s="1" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="B7" s="1" t="n">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="C7" s="1" t="n">
+        <x:v>165000000</x:v>
+      </x:c>
+      <x:c r="D7" s="1" t="n">
+        <x:v>188020017</x:v>
+      </x:c>
+      <x:c r="E7" s="1" t="n">
+        <x:v>530893735</x:v>
+      </x:c>
+      <x:c r="F7" s="1" t="n">
+        <x:v>718913752</x:v>
+      </x:c>
+    </x:row>
+  </x:sheetData>
+  <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
+  <x:pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
+  <x:headerFooter/>
+  <x:tableParts count="0"/>
+</x:worksheet>
 </file>
</xml_diff>

<commit_message>
feat: Implement exact search on movies name
Seems to pick the most popular one if there are movies with the same name.
</commit_message>
<xml_diff>
--- a/Files/Movie-Data.xlsx
+++ b/Files/Movie-Data.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <x:si>
     <x:t>Name</x:t>
   </x:si>
@@ -62,6 +62,9 @@
   </x:si>
   <x:si>
     <x:t>Interstellar</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Batman</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -401,7 +404,7 @@
   <x:dimension ref="A1"/>
   <x:sheetViews>
     <x:sheetView tabSelected="1" workbookViewId="0">
-      <x:selection activeCell="F3" sqref="F3 A1:F3"/>
+      <x:selection activeCell="F3" sqref="F3 F3:F3 A1:F3"/>
     </x:sheetView>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -554,6 +557,26 @@
         <x:v>718913752</x:v>
       </x:c>
     </x:row>
+    <x:row r="8" spans="1:6">
+      <x:c r="A8" s="1" t="s">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="B8" s="1" t="n">
+        <x:v>0.001</x:v>
+      </x:c>
+      <x:c r="C8" s="1" t="n">
+        <x:v>35000000</x:v>
+      </x:c>
+      <x:c r="D8" s="1" t="n">
+        <x:v>251409241</x:v>
+      </x:c>
+      <x:c r="E8" s="1" t="n">
+        <x:v>160160000</x:v>
+      </x:c>
+      <x:c r="F8" s="1" t="n">
+        <x:v>411569241</x:v>
+      </x:c>
+    </x:row>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
re added Files to gitignore
</commit_message>
<xml_diff>
--- a/Files/Movie-Data.xlsx
+++ b/Files/Movie-Data.xlsx
@@ -1,32 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<x:workbook xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <x:fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
+<x:workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:workbookPr codeName="ThisWorkbook"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jaskaran\Documents\UiPath\RPA-G4-2023\Files\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9C30A14-D7AA-49EF-864E-77F529D3C48B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <x:bookViews>
-    <x:workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" firstSheet="0" activeTab="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <x:workbookView firstSheet="0" activeTab="0"/>
   </x:bookViews>
   <x:sheets>
-    <x:sheet name="details" sheetId="1" r:id="rId1"/>
+    <x:sheet name="details" sheetId="2" r:id="rId2"/>
   </x:sheets>
   <x:definedNames/>
-  <x:calcPr calcId="162913"/>
-  <x:extLst>
-    <x:ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </x:ext>
-  </x:extLst>
+  <x:calcPr calcId="125725"/>
 </x:workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <x:si>
     <x:t>Name</x:t>
   </x:si>
@@ -62,26 +50,16 @@
   </x:si>
   <x:si>
     <x:t>Barbie</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Batman</x:t>
   </x:si>
 </x:sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<x:styleSheet xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x14ac x16r2 xr">
+<x:styleSheet xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:numFmts count="1">
     <x:numFmt numFmtId="0" formatCode=""/>
   </x:numFmts>
-  <x:fonts count="2" x14ac:knownFonts="1">
-    <x:font>
-      <x:sz val="11"/>
-      <x:color theme="1"/>
-      <x:name val="Calibri"/>
-      <x:family val="2"/>
-      <x:scheme val="minor"/>
-    </x:font>
+  <x:fonts count="1">
     <x:font>
       <x:vertAlign val="baseline"/>
       <x:sz val="11"/>
@@ -99,22 +77,30 @@
     </x:fill>
   </x:fills>
   <x:borders count="1">
-    <x:border>
-      <x:left/>
-      <x:right/>
-      <x:top/>
-      <x:bottom/>
-      <x:diagonal/>
+    <x:border diagonalUp="0" diagonalDown="0">
+      <x:left style="none">
+        <x:color rgb="FF000000"/>
+      </x:left>
+      <x:right style="none">
+        <x:color rgb="FF000000"/>
+      </x:right>
+      <x:top style="none">
+        <x:color rgb="FF000000"/>
+      </x:top>
+      <x:bottom style="none">
+        <x:color rgb="FF000000"/>
+      </x:bottom>
+      <x:diagonal style="none">
+        <x:color rgb="FF000000"/>
+      </x:diagonal>
     </x:border>
   </x:borders>
-  <x:cellStyleXfs count="2">
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  <x:cellStyleXfs count="1">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
   </x:cellStyleXfs>
-  <x:cellXfs count="2">
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+  <x:cellXfs count="1">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
@@ -123,19 +109,10 @@
   <x:cellStyles count="1">
     <x:cellStyle name="Normal" xfId="0" builtinId="0"/>
   </x:cellStyles>
-  <x:tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <x:extLst>
-    <x:ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </x:ext>
-    <x:ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </x:ext>
-  </x:extLst>
 </x:styleSheet>
 </file>
 
-<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/theme/theme.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
@@ -146,44 +123,44 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="44546A"/>
+        <a:srgbClr val="1F497D"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
+        <a:srgbClr val="EEECE1"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4F81BD"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="ED7D31"/>
+        <a:srgbClr val="C0504D"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
+        <a:srgbClr val="9BBB59"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="FFC000"/>
+        <a:srgbClr val="8064A2"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="4BACC6"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="70AD47"/>
+        <a:srgbClr val="F79646"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0563C1"/>
+        <a:srgbClr val="0000FF"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="954F72"/>
+        <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -210,15 +187,14 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -245,7 +221,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -257,332 +232,323 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
+                <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
   <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
-<file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xr:uid="{00000000-0001-0000-0000-000000000000}" mc:Ignorable="x14ac xr xr2 xr3">
+<file path=xl/worksheets/sheet.xml><?xml version="1.0" encoding="utf-8"?>
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:F8"/>
+  <x:dimension ref="A1:F7"/>
   <x:sheetViews>
-    <x:sheetView tabSelected="1" workbookViewId="0">
-      <x:selection activeCell="E14" sqref="E14 E14:E14"/>
-    </x:sheetView>
+    <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
-  <x:sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <x:cols>
-    <x:col min="1" max="1" width="37.285156" style="1" customWidth="1"/>
-    <x:col min="2" max="2" width="37.855469" style="1" customWidth="1"/>
-    <x:col min="3" max="3" width="22" style="1" customWidth="1"/>
-    <x:col min="4" max="4" width="34.425781" style="1" customWidth="1"/>
-    <x:col min="5" max="5" width="38.570312" style="1" customWidth="1"/>
-    <x:col min="6" max="6" width="39.570312" style="1" customWidth="1"/>
-  </x:cols>
+  <x:sheetFormatPr defaultRowHeight="15"/>
   <x:sheetData>
-    <x:row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <x:c r="A1" s="1" t="s">
+    <x:row r="1" spans="1:6">
+      <x:c r="A1" s="0" t="s">
         <x:v>0</x:v>
       </x:c>
-      <x:c r="B1" s="1" t="s">
+      <x:c r="B1" s="0" t="s">
         <x:v>1</x:v>
       </x:c>
-      <x:c r="C1" s="1" t="s">
+      <x:c r="C1" s="0" t="s">
         <x:v>2</x:v>
       </x:c>
-      <x:c r="D1" s="1" t="s">
+      <x:c r="D1" s="0" t="s">
         <x:v>3</x:v>
       </x:c>
-      <x:c r="E1" s="1" t="s">
+      <x:c r="E1" s="0" t="s">
         <x:v>4</x:v>
       </x:c>
-      <x:c r="F1" s="1" t="s">
+      <x:c r="F1" s="0" t="s">
         <x:v>5</x:v>
       </x:c>
     </x:row>
-    <x:row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <x:c r="A2" s="1" t="s">
+    <x:row r="2" spans="1:6">
+      <x:c r="A2" s="0" t="s">
         <x:v>6</x:v>
       </x:c>
-      <x:c r="B2" s="1" t="n">
+      <x:c r="B2" s="0" t="n">
         <x:v>10</x:v>
       </x:c>
-      <x:c r="C2" s="1" t="n">
+      <x:c r="C2" s="0" t="n">
         <x:v>160000000</x:v>
       </x:c>
-      <x:c r="D2" s="1" t="n">
+      <x:c r="D2" s="0" t="n">
         <x:v>292587330</x:v>
       </x:c>
-      <x:c r="E2" s="1" t="n">
+      <x:c r="E2" s="0" t="n">
         <x:v>544599280</x:v>
       </x:c>
-      <x:c r="F2" s="1" t="n">
+      <x:c r="F2" s="0" t="n">
         <x:v>837186610</x:v>
       </x:c>
     </x:row>
-    <x:row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <x:c r="A3" s="1" t="s">
+    <x:row r="3" spans="1:6">
+      <x:c r="A3" s="0" t="s">
         <x:v>7</x:v>
       </x:c>
-      <x:c r="B3" s="1" t="n">
+      <x:c r="B3" s="0" t="n">
         <x:v>7</x:v>
       </x:c>
-      <x:c r="C3" s="1" t="n">
+      <x:c r="C3" s="0" t="n">
         <x:v>72000000</x:v>
       </x:c>
-      <x:c r="D3" s="1" t="n">
+      <x:c r="D3" s="0" t="n">
         <x:v>62658220</x:v>
       </x:c>
-      <x:c r="E3" s="1" t="n">
+      <x:c r="E3" s="0" t="n">
         <x:v>34417932</x:v>
       </x:c>
-      <x:c r="F3" s="1" t="n">
+      <x:c r="F3" s="0" t="n">
         <x:v>97076152</x:v>
       </x:c>
     </x:row>
-    <x:row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <x:c r="A4" s="1" t="s">
+    <x:row r="4" spans="1:6">
+      <x:c r="A4" s="0" t="s">
         <x:v>8</x:v>
       </x:c>
-      <x:c r="B4" s="1" t="n">
+      <x:c r="B4" s="0" t="n">
         <x:v>9</x:v>
       </x:c>
-      <x:c r="C4" s="1" t="n">
+      <x:c r="C4" s="0" t="n">
         <x:v>225000000</x:v>
       </x:c>
-      <x:c r="D4" s="1" t="n">
+      <x:c r="D4" s="0" t="n">
         <x:v>291045518</x:v>
       </x:c>
-      <x:c r="E4" s="1" t="n">
+      <x:c r="E4" s="0" t="n">
         <x:v>377000000</x:v>
       </x:c>
-      <x:c r="F4" s="1" t="n">
+      <x:c r="F4" s="0" t="n">
         <x:v>668045518</x:v>
       </x:c>
     </x:row>
-    <x:row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <x:c r="A5" s="1" t="s">
+    <x:row r="5" spans="1:6">
+      <x:c r="A5" s="0" t="s">
         <x:v>9</x:v>
       </x:c>
-      <x:c r="B5" s="1" t="n">
+      <x:c r="B5" s="0" t="n">
         <x:v>2</x:v>
       </x:c>
-      <x:c r="C5" s="1" t="n">
+      <x:c r="C5" s="0" t="n">
         <x:v>-1</x:v>
       </x:c>
-      <x:c r="D5" s="1" t="n">
+      <x:c r="D5" s="0" t="n">
         <x:v>-1</x:v>
       </x:c>
-      <x:c r="E5" s="1" t="n">
+      <x:c r="E5" s="0" t="n">
         <x:v>-1</x:v>
       </x:c>
-      <x:c r="F5" s="1" t="n">
+      <x:c r="F5" s="0" t="n">
         <x:v>-1</x:v>
       </x:c>
     </x:row>
-    <x:row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <x:c r="A6" s="1" t="s">
+    <x:row r="6" spans="1:6">
+      <x:c r="A6" s="0" t="s">
         <x:v>10</x:v>
       </x:c>
-      <x:c r="B6" s="1" t="n">
+      <x:c r="B6" s="0" t="n">
         <x:v>9.5</x:v>
       </x:c>
-      <x:c r="C6" s="1" t="n">
+      <x:c r="C6" s="0" t="n">
         <x:v>220000000</x:v>
       </x:c>
-      <x:c r="D6" s="1" t="n">
+      <x:c r="D6" s="0" t="n">
         <x:v>623357910</x:v>
       </x:c>
-      <x:c r="E6" s="1" t="n">
+      <x:c r="E6" s="0" t="n">
         <x:v>897180626</x:v>
       </x:c>
-      <x:c r="F6" s="1" t="n">
+      <x:c r="F6" s="0" t="n">
         <x:v>1520538536</x:v>
       </x:c>
     </x:row>
-    <x:row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <x:c r="A7" s="1" t="s">
+    <x:row r="7" spans="1:6">
+      <x:c r="A7" s="0" t="s">
         <x:v>11</x:v>
       </x:c>
-      <x:c r="B7" s="1" t="n">
+      <x:c r="B7" s="0" t="n">
         <x:v>1</x:v>
       </x:c>
-      <x:c r="C7" s="1" t="n">
+      <x:c r="C7" s="0" t="n">
         <x:v>-1</x:v>
       </x:c>
-      <x:c r="D7" s="1" t="n">
+      <x:c r="D7" s="0" t="n">
         <x:v>601384000</x:v>
       </x:c>
-      <x:c r="E7" s="1" t="n">
+      <x:c r="E7" s="0" t="n">
         <x:v>747600000</x:v>
       </x:c>
-      <x:c r="F7" s="1" t="n">
+      <x:c r="F7" s="0" t="n">
         <x:v>1348984000</x:v>
       </x:c>
-    </x:row>
-    <x:row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <x:c r="A8" s="1" t="s">
-        <x:v>12</x:v>
-      </x:c>
-      <x:c r="B8" s="1" t="n">
-        <x:v>0.001</x:v>
-      </x:c>
-      <x:c r="C8" s="1" t="n">
-        <x:v>35000000</x:v>
-      </x:c>
-      <x:c r="D8" s="1" t="n">
-        <x:v>251409241</x:v>
-      </x:c>
-      <x:c r="E8" s="1" t="n">
-        <x:v>160160000</x:v>
-      </x:c>
-      <x:c r="F8" s="1" t="n">
-        <x:v>411569241</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="14" spans="1:6">
-      <x:c r="E14" s="1" t="s"/>
     </x:row>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
-  <x:pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
   <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
   <x:headerFooter/>
   <x:tableParts count="0"/>

</xml_diff>